<commit_message>
Corrected wrong print in the middle of the game
</commit_message>
<xml_diff>
--- a/your-code/flow.xlsx
+++ b/your-code/flow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z003yt8j\Documents\IronHack\Github\python-project\your-code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{404B67F6-DEA9-40C1-B269-FC7617E46EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63D7FC5-1F1C-47D3-8189-4F2CD9147315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{1F23A9BA-F9B2-4666-A1CD-0879F9B8B44A}"/>
+    <workbookView xWindow="7995" yWindow="1080" windowWidth="21135" windowHeight="11385" xr2:uid="{1F23A9BA-F9B2-4666-A1CD-0879F9B8B44A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -226,11 +226,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,7 +548,7 @@
   <dimension ref="C1:AG23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="F12" sqref="F12:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +567,7 @@
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
-      <c r="J2" s="13"/>
+      <c r="J2" s="12"/>
       <c r="K2" s="2"/>
       <c r="L2" s="1"/>
       <c r="M2" s="2"/>
@@ -793,9 +793,9 @@
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
@@ -813,19 +813,19 @@
       <c r="C13" s="1"/>
       <c r="D13" s="2"/>
       <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="11" t="s">
+      <c r="F13" s="14"/>
+      <c r="G13" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="11"/>
+      <c r="H13" s="14"/>
       <c r="I13" s="11"/>
-      <c r="J13" s="13"/>
+      <c r="J13" s="12"/>
       <c r="K13" s="2"/>
       <c r="L13" s="1"/>
       <c r="M13" s="2"/>
       <c r="N13" s="11"/>
       <c r="O13" s="11"/>
-      <c r="P13" s="14" t="s">
+      <c r="P13" s="13" t="s">
         <v>10</v>
       </c>
       <c r="Q13" s="11"/>

</xml_diff>